<commit_message>
trovata la libreria che crea il calendario e genera il file excel, devo vedere come manipolarle per bene e devo farmi rispedire la mail da Matteone con il modello che vuole che utilizzi
</commit_message>
<xml_diff>
--- a/windows_form_app/TEST_EXCEL.xlsx
+++ b/windows_form_app/TEST_EXCEL.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R5cbbd5f1acbe483d"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R3d6887af4b3b4aa2"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -369,8 +369,8 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
     <x:row r="1">
-      <x:c r="A1" t="b">
-        <x:v>1</x:v>
+      <x:c r="A1">
+        <x:v>39403.2118634838</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
@@ -436,8 +436,65 @@
       </x:c>
     </x:row>
     <x:row r="3">
+      <x:c r="A3">
+        <x:v>39375</x:v>
+      </x:c>
       <x:c r="B3">
-        <x:v>3.14159</x:v>
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="C3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="D3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="E3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="F3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="G3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="H3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="I3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="J3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="K3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="L3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="M3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="N3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="O3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="P3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="Q3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="R3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="S3">
+        <x:v>39375</x:v>
+      </x:c>
+      <x:c r="T3">
+        <x:v>39375</x:v>
       </x:c>
     </x:row>
     <x:row r="4">

</xml_diff>